<commit_message>
[3DBroadCastSales]-Script_Result.xlsx added to the program,Auto update as per test result
</commit_message>
<xml_diff>
--- a/Resources/[3DBroadCastSales]-Script_Result.xlsx
+++ b/Resources/[3DBroadCastSales]-Script_Result.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="40">
   <si>
     <t>Sr. No</t>
   </si>
@@ -135,10 +135,10 @@
     <t>fggo</t>
   </si>
   <si>
+    <t>Failed</t>
+  </si>
+  <si>
     <t>Pass</t>
-  </si>
-  <si>
-    <t>Failed</t>
   </si>
 </sst>
 </file>
@@ -575,15 +575,24 @@
     <xf numFmtId="0" fontId="14" fillId="13" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="14" fillId="11" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="13" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -593,15 +602,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="14" fillId="11" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1063,120 +1063,120 @@
       <c r="A2" s="38"/>
       <c r="B2" s="39"/>
       <c r="C2" s="39"/>
-      <c r="D2" s="27"/>
+      <c r="D2" s="24"/>
     </row>
     <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="B3" s="33" t="s">
+      <c r="B3" s="28" t="s">
         <v>20</v>
       </c>
-      <c r="C3" s="24"/>
-      <c r="D3" s="25"/>
+      <c r="C3" s="26"/>
+      <c r="D3" s="27"/>
     </row>
     <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="23" t="s">
+      <c r="B4" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="24"/>
-      <c r="D4" s="25"/>
+      <c r="C4" s="26"/>
+      <c r="D4" s="27"/>
     </row>
     <row r="5" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="B5" s="23" t="s">
+      <c r="B5" s="29" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="24"/>
-      <c r="D5" s="25"/>
+      <c r="C5" s="26"/>
+      <c r="D5" s="27"/>
     </row>
     <row r="6" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="B6" s="23" t="s">
+      <c r="B6" s="29" t="s">
         <v>25</v>
       </c>
-      <c r="C6" s="24"/>
-      <c r="D6" s="25"/>
+      <c r="C6" s="26"/>
+      <c r="D6" s="27"/>
     </row>
     <row r="7" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="B7" s="34" t="s">
+      <c r="B7" s="30" t="s">
         <v>27</v>
       </c>
-      <c r="C7" s="24"/>
-      <c r="D7" s="25"/>
+      <c r="C7" s="26"/>
+      <c r="D7" s="27"/>
     </row>
     <row r="8" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="B8" s="23" t="s">
+      <c r="B8" s="29" t="s">
         <v>29</v>
       </c>
-      <c r="C8" s="24"/>
-      <c r="D8" s="25"/>
+      <c r="C8" s="26"/>
+      <c r="D8" s="27"/>
     </row>
     <row r="9" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="B9" s="23" t="s">
+      <c r="B9" s="29" t="s">
         <v>31</v>
       </c>
-      <c r="C9" s="24"/>
-      <c r="D9" s="25"/>
+      <c r="C9" s="26"/>
+      <c r="D9" s="27"/>
     </row>
     <row r="10" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="11" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="12" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="13" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="32" t="s">
+      <c r="A13" s="25" t="s">
         <v>32</v>
       </c>
-      <c r="B13" s="24"/>
-      <c r="C13" s="24"/>
-      <c r="D13" s="24"/>
-      <c r="E13" s="24"/>
-      <c r="F13" s="25"/>
+      <c r="B13" s="26"/>
+      <c r="C13" s="26"/>
+      <c r="D13" s="26"/>
+      <c r="E13" s="26"/>
+      <c r="F13" s="27"/>
     </row>
     <row r="14" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="29" t="s">
+      <c r="A14" s="32" t="s">
         <v>33</v>
       </c>
-      <c r="B14" s="26" t="s">
+      <c r="B14" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="C14" s="26" t="s">
+      <c r="C14" s="23" t="s">
         <v>34</v>
       </c>
-      <c r="D14" s="31" t="s">
+      <c r="D14" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="E14" s="27"/>
-      <c r="F14" s="26" t="s">
+      <c r="E14" s="24"/>
+      <c r="F14" s="23" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="30"/>
-      <c r="B15" s="27"/>
-      <c r="C15" s="27"/>
+      <c r="A15" s="33"/>
+      <c r="B15" s="24"/>
+      <c r="C15" s="24"/>
       <c r="D15" s="18" t="s">
         <v>35</v>
       </c>
       <c r="E15" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="F15" s="27"/>
+      <c r="F15" s="24"/>
     </row>
     <row r="16" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="19">
@@ -1203,10 +1203,10 @@
       </c>
     </row>
     <row r="17" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="28" t="s">
+      <c r="A17" s="31" t="s">
         <v>15</v>
       </c>
-      <c r="B17" s="27"/>
+      <c r="B17" s="24"/>
       <c r="C17" s="22">
         <f t="shared" ref="C17:F17" si="0">SUM(C16)</f>
         <v>3</v>
@@ -2213,6 +2213,10 @@
     <row r="1000" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="D14:E14"/>
     <mergeCell ref="A1:D2"/>
     <mergeCell ref="B5:D5"/>
     <mergeCell ref="B4:D4"/>
@@ -2224,10 +2228,6 @@
     <mergeCell ref="B8:D8"/>
     <mergeCell ref="B9:D9"/>
     <mergeCell ref="B14:B15"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="A14:A15"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="D14:E14"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B7" r:id="rId1"/>
@@ -2299,7 +2299,7 @@
         <v>6</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="63.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2313,7 +2313,7 @@
         <v>6</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>39</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2325,7 +2325,7 @@
       <c r="A10" s="40" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="25"/>
+      <c r="B10" s="27"/>
       <c r="C10" s="8" t="s">
         <v>12</v>
       </c>
@@ -2340,7 +2340,7 @@
       </c>
       <c r="C11" s="11">
         <f>COUNTIF(D2:D38,"Pass")</f>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2353,7 +2353,7 @@
       </c>
       <c r="C12" s="11">
         <f>COUNTIF(D2:D38,"Failed")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2361,12 +2361,12 @@
         <v>14</v>
       </c>
       <c r="B13" s="10">
-        <f t="shared" ref="B13:C13" si="0">COUNTIF(C2:C38,"Skipped")</f>
+        <f t="shared" ref="B13" si="0">COUNTIF(C2:C38,"Skipped")</f>
         <v>0</v>
       </c>
       <c r="C13" s="14">
         <f>COUNTIF(D2:D38,"Skipped")</f>
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Test case 4 partly finished
</commit_message>
<xml_diff>
--- a/Resources/[3DBroadCastSales]-Script_Result.xlsx
+++ b/Resources/[3DBroadCastSales]-Script_Result.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="41">
   <si>
     <t>Sr. No</t>
   </si>
@@ -135,7 +135,10 @@
     <t>fggo</t>
   </si>
   <si>
-    <t>Failed</t>
+    <t>TC_Menu_Page_04</t>
+  </si>
+  <si>
+    <t>Verify User is able to add/remove the Products into "Wish List" and "Compare List"</t>
   </si>
   <si>
     <t>Pass</t>
@@ -146,7 +149,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -225,6 +228,12 @@
       <b/>
       <sz val="11"/>
       <name val="Cambria"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Cambria"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="14">
@@ -507,7 +516,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -613,11 +622,71 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="12">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFF2CC"/>
+          <bgColor rgb="FFFFF2CC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4CCCC"/>
+          <bgColor rgb="FFF4CCCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFD9EAD3"/>
+          <bgColor rgb="FFD9EAD3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF990000"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4CCCC"/>
+          <bgColor rgb="FFF4CCCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFBF9000"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFF2CC"/>
+          <bgColor rgb="FFFFF2CC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF38761D"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFD9EAD3"/>
+          <bgColor rgb="FFD9EAD3"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -1187,11 +1256,11 @@
       </c>
       <c r="C16" s="21">
         <f>Dashboard!B14</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D16" s="21">
         <f>Dashboard!B11</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E16" s="21">
         <f>Dashboard!B12</f>
@@ -1209,11 +1278,11 @@
       <c r="B17" s="24"/>
       <c r="C17" s="22">
         <f t="shared" ref="C17:F17" si="0">SUM(C16)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D17" s="22">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E17" s="22">
         <f t="shared" si="0"/>
@@ -2246,13 +2315,13 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D4" sqref="D4"/>
+      <selection pane="bottomLeft" activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="13.42578125" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="41.28515625" collapsed="true"/>
+    <col min="1" max="1" customWidth="true" width="15.5703125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="69.28515625" collapsed="true"/>
     <col min="3" max="3" customWidth="true" width="20.140625" collapsed="true"/>
     <col min="4" max="4" customWidth="true" width="14.28515625" collapsed="true"/>
   </cols>
@@ -2282,7 +2351,7 @@
         <v>6</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>39</v>
+        <v>14</v>
       </c>
       <c r="E2" s="7"/>
       <c r="F2" s="7"/>
@@ -2299,10 +2368,10 @@
         <v>6</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>39</v>
+        <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="63.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" ht="53.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>9</v>
       </c>
@@ -2313,10 +2382,23 @@
         <v>6</v>
       </c>
       <c r="D4" s="6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
         <v>38</v>
       </c>
+      <c r="B5" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2336,11 +2418,11 @@
       </c>
       <c r="B11" s="10">
         <f>COUNTIF(C2:C38,"Automated")</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C11" s="11">
         <f>COUNTIF(D2:D38,"Pass")</f>
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2353,7 +2435,7 @@
       </c>
       <c r="C12" s="11">
         <f>COUNTIF(D2:D38,"Failed")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2366,7 +2448,7 @@
       </c>
       <c r="C13" s="14">
         <f>COUNTIF(D2:D38,"Skipped")</f>
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2375,11 +2457,11 @@
       </c>
       <c r="B14" s="16">
         <f t="shared" ref="B14" si="1">SUM(B11:B13)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C14" s="16">
         <f>SUM(C11:C13)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3372,44 +3454,45 @@
   <mergeCells count="1">
     <mergeCell ref="A10:B10"/>
   </mergeCells>
-  <conditionalFormatting sqref="C2:C4">
-    <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
+  <conditionalFormatting sqref="C2:C5">
+    <cfRule type="cellIs" dxfId="11" priority="1" operator="equal">
       <formula>"Automated"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C2:C4">
-    <cfRule type="containsText" dxfId="4" priority="2" operator="containsText" text="Skipped">
+  <conditionalFormatting sqref="C2:C5">
+    <cfRule type="containsText" dxfId="10" priority="2" operator="containsText" text="Skipped">
       <formula>NOT(ISERROR(SEARCH(("Skipped"),(C2))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C2:C4">
-    <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="NotAutomated">
+  <conditionalFormatting sqref="C2:C5">
+    <cfRule type="containsText" dxfId="9" priority="3" operator="containsText" text="NotAutomated">
       <formula>NOT(ISERROR(SEARCH(("NotAutomated"),(C2))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D2:D4">
-    <cfRule type="containsText" dxfId="2" priority="4" operator="containsText" text="Pass">
+  <conditionalFormatting sqref="D2:D5">
+    <cfRule type="containsText" dxfId="8" priority="4" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH(("Pass"),(D2))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D2:D4">
-    <cfRule type="containsText" dxfId="1" priority="5" operator="containsText" text="Failed">
+  <conditionalFormatting sqref="D2:D5">
+    <cfRule type="containsText" dxfId="7" priority="5" operator="containsText" text="Failed">
       <formula>NOT(ISERROR(SEARCH(("Failed"),(D2))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D2:D4">
-    <cfRule type="containsText" dxfId="0" priority="6" operator="containsText" text="Skipped">
+  <conditionalFormatting sqref="D2:D5">
+    <cfRule type="containsText" dxfId="6" priority="6" operator="containsText" text="Skipped">
       <formula>NOT(ISERROR(SEARCH(("Skipped"),(D2))))</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" sqref="C2:C4">
+    <dataValidation type="list" allowBlank="1" sqref="C2:C5">
       <formula1>"Automated,Skipped,NotAutomated"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="D2:D4">
+    <dataValidation type="list" allowBlank="1" sqref="D2:D5">
       <formula1>"Pass,Failed,Skipped"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>